<commit_message>
Add benchmarks and score function
</commit_message>
<xml_diff>
--- a/database/antigens/test_antigens_summary.xlsx
+++ b/database/antigens/test_antigens_summary.xlsx
@@ -12,6 +12,9 @@
     <sheet name="nerve_1_tests" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="nerve_2_tests" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">nerve_2_tests!$A$1:$L$108</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -2532,6 +2535,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2540,10 +2547,10 @@
   <dimension ref="A1:L317"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A280" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A296" activeCellId="1" sqref="J2:J20 A296"/>
+      <selection pane="topLeft" activeCell="A296" activeCellId="1" sqref="I21:I55 A296"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -11827,10 +11834,10 @@
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="J2:J20 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="I21:I55 G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -14185,16 +14192,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21:I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.62"/>
@@ -14226,10 +14233,10 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -14239,7 +14246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>133</v>
       </c>
@@ -14274,7 +14281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>133</v>
       </c>
@@ -15592,7 +15599,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>599</v>
       </c>
@@ -15627,7 +15634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>599</v>
       </c>
@@ -15662,7 +15669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>606</v>
       </c>
@@ -15697,7 +15704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>611</v>
       </c>
@@ -16117,7 +16124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>663</v>
       </c>
@@ -16152,7 +16159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>668</v>
       </c>
@@ -16187,7 +16194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>674</v>
       </c>
@@ -16222,7 +16229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>674</v>
       </c>
@@ -16257,7 +16264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>674</v>
       </c>
@@ -16292,7 +16299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>674</v>
       </c>
@@ -16327,7 +16334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>674</v>
       </c>
@@ -16362,7 +16369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>674</v>
       </c>
@@ -16397,7 +16404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>674</v>
       </c>
@@ -16432,7 +16439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>674</v>
       </c>
@@ -16467,7 +16474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>674</v>
       </c>
@@ -16502,7 +16509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>674</v>
       </c>
@@ -16537,7 +16544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>674</v>
       </c>
@@ -16572,7 +16579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>674</v>
       </c>
@@ -16607,7 +16614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>674</v>
       </c>
@@ -16642,7 +16649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>674</v>
       </c>
@@ -16677,7 +16684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>711</v>
       </c>
@@ -16712,7 +16719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>711</v>
       </c>
@@ -16747,7 +16754,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>711</v>
       </c>
@@ -16782,7 +16789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>711</v>
       </c>
@@ -16817,7 +16824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>674</v>
       </c>
@@ -16852,7 +16859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>711</v>
       </c>
@@ -16887,7 +16894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>711</v>
       </c>
@@ -16922,7 +16929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>711</v>
       </c>
@@ -16957,7 +16964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>711</v>
       </c>
@@ -16992,7 +16999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>711</v>
       </c>
@@ -17027,7 +17034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>711</v>
       </c>
@@ -17062,7 +17069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>737</v>
       </c>
@@ -17482,7 +17489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>774</v>
       </c>
@@ -17517,7 +17524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>778</v>
       </c>
@@ -17552,7 +17559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>555</v>
       </c>
@@ -17587,7 +17594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>784</v>
       </c>
@@ -17622,7 +17629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>788</v>
       </c>
@@ -17657,7 +17664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>788</v>
       </c>
@@ -17692,7 +17699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>784</v>
       </c>
@@ -17727,7 +17734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>788</v>
       </c>
@@ -17762,7 +17769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>798</v>
       </c>
@@ -17797,7 +17804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>798</v>
       </c>
@@ -17973,6 +17980,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L108">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="-"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -17980,5 +17994,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>